<commit_message>
added debugging for token error and corrected corruption of enhanced report generation
</commit_message>
<xml_diff>
--- a/who_test_controls_analysis_results.xlsx
+++ b/who_test_controls_analysis_results.xlsx
@@ -1357,21 +1357,9 @@
       <c r="A2" t="n">
         <v>12651</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
           <t>None</t>
@@ -1387,71 +1375,43 @@
       <c r="A3" t="n">
         <v>11102</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>6463</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>7140</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
@@ -1467,26 +1427,14 @@
           <t>None</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>10575</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>Replace weak verb 'performs' with a stronger control verb like 'verify', 'examine', or 'evaluate'; Consider using active voice to clearly indicate responsibility for control activities.</t>
@@ -1497,21 +1445,13 @@
           <t>None</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>4645</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
@@ -1537,16 +1477,8 @@
       <c r="A8" t="n">
         <v>4310</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>Consider using active voice to clearly indicate who performs the control; Consider clarifying the object of 'review' to be more specific.; Consider using active voice to clearly indicate responsibility for control activities.</t>
@@ -1557,26 +1489,14 @@
           <t>None</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>3867</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
           <t>Consider clarifying the object of 'relate' to be more specific.; Consider using active voice to clearly indicate responsibility for control activities.</t>
@@ -1587,11 +1507,7 @@
           <t>None</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1612,10 +1528,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="13.2" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="7.700000000000001" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1670,7 +1586,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-facing materials must be reviewed</t>
+          <t>'-facing materials must be reviewed</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1940,7 +1856,7 @@
       <c r="B19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Top Vague Terms</t>
         </is>
@@ -2041,7 +1957,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>This analysis evaluates control descriptions based on seven key elements that should be present in a well-written control description:</t>
+          <t>This analysis evaluates control descriptions based on five key elements that should be present in a well-written control description:</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -2307,7 +2223,7 @@
       <c r="B41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="inlineStr">
+      <c r="A42" t="inlineStr">
         <is>
           <t>Enhanced Validation Checks</t>
         </is>

</xml_diff>